<commit_message>
scan manager fix save logs v1
</commit_message>
<xml_diff>
--- a/history-2025-12-17.xlsx
+++ b/history-2025-12-17.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -443,7 +443,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B2" t="str">
-        <v>16:27:56</v>
+        <v>16:38:04</v>
       </c>
       <c r="F2" t="str">
         <v>227028-8400</v>
@@ -452,7 +452,7 @@
         <v/>
       </c>
       <c r="H2" t="str">
-        <v>MATCHED_FIELD</v>
+        <v>ALL_FIELDS_MATCHED</v>
       </c>
     </row>
     <row r="3">
@@ -460,16 +460,16 @@
         <v>17/12/2025</v>
       </c>
       <c r="B3" t="str">
-        <v>16:27:53</v>
+        <v>16:37:57</v>
       </c>
       <c r="F3" t="str">
-        <v>UL1569AWG22RED/BLACK(BARE)</v>
+        <v>227028-8400</v>
       </c>
       <c r="G3" t="str">
         <v/>
       </c>
       <c r="H3" t="str">
-        <v>MATCHED_FIELD</v>
+        <v>ALL_FIELDS_MATCHED</v>
       </c>
     </row>
     <row r="4">
@@ -477,7 +477,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B4" t="str">
-        <v>16:27:41</v>
+        <v>16:37:48</v>
       </c>
       <c r="F4" t="str">
         <v>227028-8400</v>
@@ -494,7 +494,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B5" t="str">
-        <v>16:27:41</v>
+        <v>16:37:39</v>
       </c>
       <c r="F5" t="str">
         <v>227028-8400</v>
@@ -503,7 +503,7 @@
         <v/>
       </c>
       <c r="H5" t="str">
-        <v>MATCHED_FIELD</v>
+        <v>ALL_FIELDS_MATCHED</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B6" t="str">
-        <v>16:27:40</v>
+        <v>16:27:56</v>
       </c>
       <c r="F6" t="str">
         <v>227028-8400</v>
@@ -528,7 +528,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B7" t="str">
-        <v>16:27:38</v>
+        <v>16:27:53</v>
       </c>
       <c r="F7" t="str">
         <v>UL1569AWG22RED/BLACK(BARE)</v>
@@ -545,7 +545,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B8" t="str">
-        <v>16:25:43</v>
+        <v>16:27:41</v>
       </c>
       <c r="F8" t="str">
         <v>227028-8400</v>
@@ -562,7 +562,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B9" t="str">
-        <v>16:25:43</v>
+        <v>16:27:41</v>
       </c>
       <c r="F9" t="str">
         <v>227028-8400</v>
@@ -579,7 +579,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B10" t="str">
-        <v>16:25:41</v>
+        <v>16:27:40</v>
       </c>
       <c r="F10" t="str">
         <v>227028-8400</v>
@@ -596,7 +596,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B11" t="str">
-        <v>16:25:40</v>
+        <v>16:27:38</v>
       </c>
       <c r="F11" t="str">
         <v>UL1569AWG22RED/BLACK(BARE)</v>
@@ -613,7 +613,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B12" t="str">
-        <v>16:22:41</v>
+        <v>16:25:43</v>
       </c>
       <c r="F12" t="str">
         <v>227028-8400</v>
@@ -630,7 +630,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B13" t="str">
-        <v>16:22:41</v>
+        <v>16:25:43</v>
       </c>
       <c r="F13" t="str">
         <v>227028-8400</v>
@@ -647,7 +647,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B14" t="str">
-        <v>16:22:40</v>
+        <v>16:25:41</v>
       </c>
       <c r="F14" t="str">
         <v>227028-8400</v>
@@ -664,7 +664,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B15" t="str">
-        <v>16:22:39</v>
+        <v>16:25:40</v>
       </c>
       <c r="F15" t="str">
         <v>UL1569AWG22RED/BLACK(BARE)</v>
@@ -681,7 +681,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B16" t="str">
-        <v>16:22:36</v>
+        <v>16:22:41</v>
       </c>
       <c r="F16" t="str">
         <v>227028-8400</v>
@@ -698,7 +698,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B17" t="str">
-        <v>16:22:36</v>
+        <v>16:22:41</v>
       </c>
       <c r="F17" t="str">
         <v>227028-8400</v>
@@ -715,7 +715,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B18" t="str">
-        <v>16:22:35</v>
+        <v>16:22:40</v>
       </c>
       <c r="F18" t="str">
         <v>227028-8400</v>
@@ -732,7 +732,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B19" t="str">
-        <v>16:22:34</v>
+        <v>16:22:39</v>
       </c>
       <c r="F19" t="str">
         <v>UL1569AWG22RED/BLACK(BARE)</v>
@@ -749,7 +749,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B20" t="str">
-        <v>16:22:32</v>
+        <v>16:22:36</v>
       </c>
       <c r="F20" t="str">
         <v>227028-8400</v>
@@ -766,7 +766,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B21" t="str">
-        <v>16:22:32</v>
+        <v>16:22:36</v>
       </c>
       <c r="F21" t="str">
         <v>227028-8400</v>
@@ -783,7 +783,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B22" t="str">
-        <v>16:22:31</v>
+        <v>16:22:35</v>
       </c>
       <c r="F22" t="str">
         <v>227028-8400</v>
@@ -800,7 +800,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B23" t="str">
-        <v>16:22:30</v>
+        <v>16:22:34</v>
       </c>
       <c r="F23" t="str">
         <v>UL1569AWG22RED/BLACK(BARE)</v>
@@ -817,7 +817,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B24" t="str">
-        <v>16:22:20</v>
+        <v>16:22:32</v>
       </c>
       <c r="F24" t="str">
         <v>227028-8400</v>
@@ -834,7 +834,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B25" t="str">
-        <v>16:22:20</v>
+        <v>16:22:32</v>
       </c>
       <c r="F25" t="str">
         <v>227028-8400</v>
@@ -851,7 +851,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B26" t="str">
-        <v>16:22:18</v>
+        <v>16:22:31</v>
       </c>
       <c r="F26" t="str">
         <v>227028-8400</v>
@@ -868,7 +868,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B27" t="str">
-        <v>16:22:16</v>
+        <v>16:22:30</v>
       </c>
       <c r="F27" t="str">
         <v>UL1569AWG22RED/BLACK(BARE)</v>
@@ -885,16 +885,16 @@
         <v>17/12/2025</v>
       </c>
       <c r="B28" t="str">
-        <v>16:20:12</v>
+        <v>16:22:20</v>
       </c>
       <c r="F28" t="str">
-        <v>UL1569AWG22RED/BLACK(BARE)</v>
+        <v>227028-8400</v>
       </c>
       <c r="G28" t="str">
         <v/>
       </c>
       <c r="H28" t="str">
-        <v>MATCHED_FIELD</v>
+        <v>ALL_FIELDS_MATCHED</v>
       </c>
     </row>
     <row r="29">
@@ -902,7 +902,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B29" t="str">
-        <v>16:11:16</v>
+        <v>16:22:20</v>
       </c>
       <c r="F29" t="str">
         <v>227028-8400</v>
@@ -919,10 +919,10 @@
         <v>17/12/2025</v>
       </c>
       <c r="B30" t="str">
-        <v>16:11:12</v>
+        <v>16:22:18</v>
       </c>
       <c r="F30" t="str">
-        <v>UL1569AWG22RED/BLACK(BARE)</v>
+        <v>227028-8400</v>
       </c>
       <c r="G30" t="str">
         <v/>
@@ -936,7 +936,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B31" t="str">
-        <v>16:08:26</v>
+        <v>16:22:16</v>
       </c>
       <c r="F31" t="str">
         <v>UL1569AWG22RED/BLACK(BARE)</v>
@@ -953,7 +953,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B32" t="str">
-        <v>16:07:53</v>
+        <v>16:20:12</v>
       </c>
       <c r="F32" t="str">
         <v>UL1569AWG22RED/BLACK(BARE)</v>
@@ -970,10 +970,10 @@
         <v>17/12/2025</v>
       </c>
       <c r="B33" t="str">
-        <v>16:06:10</v>
+        <v>16:11:16</v>
       </c>
       <c r="F33" t="str">
-        <v>UL1569AWG22RED/BLACK(BARE)</v>
+        <v>227028-8400</v>
       </c>
       <c r="G33" t="str">
         <v/>
@@ -987,7 +987,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B34" t="str">
-        <v>16:00:21</v>
+        <v>16:11:12</v>
       </c>
       <c r="F34" t="str">
         <v>UL1569AWG22RED/BLACK(BARE)</v>
@@ -1004,7 +1004,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B35" t="str">
-        <v>15:12:54</v>
+        <v>16:08:26</v>
       </c>
       <c r="F35" t="str">
         <v>UL1569AWG22RED/BLACK(BARE)</v>
@@ -1013,7 +1013,7 @@
         <v/>
       </c>
       <c r="H35" t="str">
-        <v>ALL_FIELDS_MATCHED</v>
+        <v>MATCHED_FIELD</v>
       </c>
     </row>
     <row r="36">
@@ -1021,7 +1021,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B36" t="str">
-        <v>15:12:54</v>
+        <v>16:07:53</v>
       </c>
       <c r="F36" t="str">
         <v>UL1569AWG22RED/BLACK(BARE)</v>
@@ -1038,7 +1038,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B37" t="str">
-        <v>15:10:44</v>
+        <v>16:06:10</v>
       </c>
       <c r="F37" t="str">
         <v>UL1569AWG22RED/BLACK(BARE)</v>
@@ -1047,7 +1047,7 @@
         <v/>
       </c>
       <c r="H37" t="str">
-        <v>ALL_FIELDS_MATCHED</v>
+        <v>MATCHED_FIELD</v>
       </c>
     </row>
     <row r="38">
@@ -1055,7 +1055,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B38" t="str">
-        <v>15:10:44</v>
+        <v>16:00:21</v>
       </c>
       <c r="F38" t="str">
         <v>UL1569AWG22RED/BLACK(BARE)</v>
@@ -1072,7 +1072,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B39" t="str">
-        <v>15:08:22</v>
+        <v>15:12:54</v>
       </c>
       <c r="F39" t="str">
         <v>UL1569AWG22RED/BLACK(BARE)</v>
@@ -1089,7 +1089,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B40" t="str">
-        <v>15:08:22</v>
+        <v>15:12:54</v>
       </c>
       <c r="F40" t="str">
         <v>UL1569AWG22RED/BLACK(BARE)</v>
@@ -1106,7 +1106,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B41" t="str">
-        <v>14:55:13</v>
+        <v>15:10:44</v>
       </c>
       <c r="F41" t="str">
         <v>UL1569AWG22RED/BLACK(BARE)</v>
@@ -1123,7 +1123,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B42" t="str">
-        <v>14:55:13</v>
+        <v>15:10:44</v>
       </c>
       <c r="F42" t="str">
         <v>UL1569AWG22RED/BLACK(BARE)</v>
@@ -1140,7 +1140,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B43" t="str">
-        <v>14:52:03</v>
+        <v>15:08:22</v>
       </c>
       <c r="F43" t="str">
         <v>UL1569AWG22RED/BLACK(BARE)</v>
@@ -1157,7 +1157,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B44" t="str">
-        <v>14:52:03</v>
+        <v>15:08:22</v>
       </c>
       <c r="F44" t="str">
         <v>UL1569AWG22RED/BLACK(BARE)</v>
@@ -1174,7 +1174,7 @@
         <v>17/12/2025</v>
       </c>
       <c r="B45" t="str">
-        <v>14:50:28</v>
+        <v>14:55:13</v>
       </c>
       <c r="F45" t="str">
         <v>UL1569AWG22RED/BLACK(BARE)</v>
@@ -1191,21 +1191,89 @@
         <v>17/12/2025</v>
       </c>
       <c r="B46" t="str">
+        <v>14:55:13</v>
+      </c>
+      <c r="F46" t="str">
+        <v>UL1569AWG22RED/BLACK(BARE)</v>
+      </c>
+      <c r="G46" t="str">
+        <v/>
+      </c>
+      <c r="H46" t="str">
+        <v>MATCHED_FIELD</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="B47" t="str">
+        <v>14:52:03</v>
+      </c>
+      <c r="F47" t="str">
+        <v>UL1569AWG22RED/BLACK(BARE)</v>
+      </c>
+      <c r="G47" t="str">
+        <v/>
+      </c>
+      <c r="H47" t="str">
+        <v>ALL_FIELDS_MATCHED</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="B48" t="str">
+        <v>14:52:03</v>
+      </c>
+      <c r="F48" t="str">
+        <v>UL1569AWG22RED/BLACK(BARE)</v>
+      </c>
+      <c r="G48" t="str">
+        <v/>
+      </c>
+      <c r="H48" t="str">
+        <v>MATCHED_FIELD</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="B49" t="str">
         <v>14:50:28</v>
       </c>
-      <c r="F46" t="str">
-        <v>UL1569AWG22RED/BLACK(BARE)</v>
-      </c>
-      <c r="G46" t="str">
-        <v/>
-      </c>
-      <c r="H46" t="str">
+      <c r="F49" t="str">
+        <v>UL1569AWG22RED/BLACK(BARE)</v>
+      </c>
+      <c r="G49" t="str">
+        <v/>
+      </c>
+      <c r="H49" t="str">
+        <v>ALL_FIELDS_MATCHED</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="B50" t="str">
+        <v>14:50:28</v>
+      </c>
+      <c r="F50" t="str">
+        <v>UL1569AWG22RED/BLACK(BARE)</v>
+      </c>
+      <c r="G50" t="str">
+        <v/>
+      </c>
+      <c r="H50" t="str">
         <v>MATCHED_FIELD</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H46"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H50"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>